<commit_message>
Added final library version
</commit_message>
<xml_diff>
--- a/Docs/Process_Document.xlsx
+++ b/Docs/Process_Document.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Specs__goals">Sheet1!$E$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>10.04.2019</t>
   </si>
@@ -86,9 +89,6 @@
     <t>2x 2N2222 TRANSISTORS</t>
   </si>
   <si>
-    <t>Timeline</t>
-  </si>
-  <si>
     <t>Specs (goals)</t>
   </si>
   <si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>Release Candidate</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>MILESTONE</t>
+  </si>
+  <si>
+    <t>TIMELINE</t>
+  </si>
+  <si>
+    <t>Improve features</t>
   </si>
 </sst>
 </file>
@@ -223,14 +235,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -241,6 +291,41 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D1:F6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="D1:F6"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Specs (goals)"/>
+    <tableColumn id="2" name="Project design"/>
+    <tableColumn id="3" name="Implementation "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D8:F13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D8:F13"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Testing (Automated + Manual)"/>
+    <tableColumn id="2" name="Bugfixing + Improvements"/>
+    <tableColumn id="3" name="RELEASE DoD (Definition of Done)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:B10" totalsRowShown="0">
+  <autoFilter ref="A2:B10"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="DATE"/>
+    <tableColumn id="2" name="MILESTONE"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,15 +591,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
     <col min="4" max="4" width="63" customWidth="1"/>
@@ -524,217 +609,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="D1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>43</v>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>